<commit_message>
Update Machine Learning Courses.xlsx
</commit_message>
<xml_diff>
--- a/Track - Machine Learning/Machine Learning Courses.xlsx
+++ b/Track - Machine Learning/Machine Learning Courses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="140">
   <si>
     <t>Source</t>
   </si>
@@ -297,6 +297,153 @@
   </si>
   <si>
     <t>But What Do the Nuns Think?</t>
+  </si>
+  <si>
+    <t>StatQuest</t>
+  </si>
+  <si>
+    <t>ML Fundamentals: Cross Validation</t>
+  </si>
+  <si>
+    <t>A Gentle Introduction to ML</t>
+  </si>
+  <si>
+    <t>ML Fundamentals: Confusion Matrix</t>
+  </si>
+  <si>
+    <t>ML Fundamentals: Sensitivity and Specificity</t>
+  </si>
+  <si>
+    <t>ML Fundamentals: Bias and Variance</t>
+  </si>
+  <si>
+    <t>ROC and AUC, Clearly Explained!</t>
+  </si>
+  <si>
+    <t>ROC and AUC in R</t>
+  </si>
+  <si>
+    <t>SQ: Fitting a line to data, aka least squares, aka linear regression</t>
+  </si>
+  <si>
+    <t>SQ: Odds and Log(Odds) Clearly Explained!!!</t>
+  </si>
+  <si>
+    <t>SQ: Odds Ratios and Log(Odds Ratios), Clearly Explained!!!</t>
+  </si>
+  <si>
+    <t>SQ: Logistic Regression</t>
+  </si>
+  <si>
+    <t>Logistic Regression Details Pt1: Coefficients</t>
+  </si>
+  <si>
+    <t>Logistic Regression Details Pt2: Maximum Likelihood</t>
+  </si>
+  <si>
+    <t>Logistic Regression Details Pt3: R-squared and p-value</t>
+  </si>
+  <si>
+    <t>Satirated Models and Deviance</t>
+  </si>
+  <si>
+    <t>Logistic Regression in R, Clearly Explained!!!</t>
+  </si>
+  <si>
+    <t>Deviance Residuals</t>
+  </si>
+  <si>
+    <t>Regularization Part 1: Ridge Regression</t>
+  </si>
+  <si>
+    <t>Regularization Part 2: Lasso Regression</t>
+  </si>
+  <si>
+    <t>Regularization Part 3: Elastic Net Regression</t>
+  </si>
+  <si>
+    <t>Ridge, Lsso and Elastic-Net Regression in R</t>
+  </si>
+  <si>
+    <t>SQ: Principal Component Analysis (PCA), Step-by-Step</t>
+  </si>
+  <si>
+    <t>SQ: PCA main ideas in only 5 minutes!!!</t>
+  </si>
+  <si>
+    <t>SQ: PCA in R</t>
+  </si>
+  <si>
+    <t>SQ: PCA in Python</t>
+  </si>
+  <si>
+    <t>SQ: Linear Discriminant Analysis (LDA) clearly explained</t>
+  </si>
+  <si>
+    <t>SQ: MDS and PCoA</t>
+  </si>
+  <si>
+    <t>SQ: MDS and PCoA in R</t>
+  </si>
+  <si>
+    <t>SQ: t-SNE, Clearly Explained</t>
+  </si>
+  <si>
+    <t>SQ: Hierarchical Clustering</t>
+  </si>
+  <si>
+    <t>SQ: K-means Clustering</t>
+  </si>
+  <si>
+    <t>SQ: K-nearest neighbors, Clearly Explained</t>
+  </si>
+  <si>
+    <t>SQ: Decision Trees</t>
+  </si>
+  <si>
+    <t>SQ: Decision Trees, Part 2 - Feature Selection and Missing Data</t>
+  </si>
+  <si>
+    <t>SQ: Random Forests Part 1 - Building, Using and Evaluating</t>
+  </si>
+  <si>
+    <t>SQ: Random Forests Part 2 - Missing data and clustering</t>
+  </si>
+  <si>
+    <t>SQ: Random Forests in R</t>
+  </si>
+  <si>
+    <t>SQ: PCA - Practical Tips</t>
+  </si>
+  <si>
+    <t>Gradient Descent, Step-by-Step</t>
+  </si>
+  <si>
+    <t>Stochastic Gradient Descent, Clearly Explained!!!</t>
+  </si>
+  <si>
+    <t>AdaBoost, Clearly Explained</t>
+  </si>
+  <si>
+    <t>Gradient Boost Part 1: Regression Main Ideas</t>
+  </si>
+  <si>
+    <t>Gradient Boost Part 2: Regression Details</t>
+  </si>
+  <si>
+    <t>Gradient Boost Part 3: Classification</t>
+  </si>
+  <si>
+    <t>Gradient Boost Part 4: Classification Details</t>
+  </si>
+  <si>
+    <t>SQ: Fitting a curve to data, aka lowess, aka loess</t>
+  </si>
+  <si>
+    <t>Statistics Fundamentals: Population Parameters</t>
+  </si>
+  <si>
+    <t>Pricipal Component Analysis (PCA) clearly explained (2015)</t>
   </si>
 </sst>
 </file>
@@ -634,7 +781,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -648,7 +795,7 @@
     <col min="3" max="3" width="61.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -658,8 +805,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -669,8 +819,11 @@
       <c r="C2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -680,8 +833,11 @@
       <c r="C3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -691,8 +847,11 @@
       <c r="C4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -702,8 +861,11 @@
       <c r="C5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -713,8 +875,11 @@
       <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -724,8 +889,11 @@
       <c r="C7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -735,8 +903,11 @@
       <c r="C8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -747,7 +918,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -757,8 +928,11 @@
       <c r="C10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -768,8 +942,11 @@
       <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -779,8 +956,11 @@
       <c r="C12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -791,7 +971,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -801,8 +981,11 @@
       <c r="C14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
@@ -812,8 +995,11 @@
       <c r="C15" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -823,8 +1009,11 @@
       <c r="C16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -834,8 +1023,11 @@
       <c r="C17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -845,8 +1037,11 @@
       <c r="C18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -856,8 +1051,11 @@
       <c r="C19" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -867,8 +1065,11 @@
       <c r="C20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -879,7 +1080,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -889,8 +1090,11 @@
       <c r="C22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -900,8 +1104,11 @@
       <c r="C23" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
@@ -911,8 +1118,11 @@
       <c r="C24" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -922,8 +1132,11 @@
       <c r="C25" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -934,7 +1147,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -944,8 +1157,11 @@
       <c r="C27" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>3</v>
       </c>
@@ -955,8 +1171,11 @@
       <c r="C28" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -966,8 +1185,11 @@
       <c r="C29" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -977,8 +1199,11 @@
       <c r="C30" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -988,8 +1213,11 @@
       <c r="C31" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
@@ -1000,7 +1228,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1010,8 +1238,11 @@
       <c r="C33" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1021,8 +1252,11 @@
       <c r="C34" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -1032,8 +1266,11 @@
       <c r="C35" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1044,7 +1281,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
@@ -1054,8 +1291,11 @@
       <c r="C37" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1065,8 +1305,11 @@
       <c r="C38" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1076,8 +1319,11 @@
       <c r="C39" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -1087,8 +1333,11 @@
       <c r="C40" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>3</v>
       </c>
@@ -1099,7 +1348,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1109,8 +1358,11 @@
       <c r="C42" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1120,8 +1372,11 @@
       <c r="C43" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1132,7 +1387,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>3</v>
       </c>
@@ -1142,8 +1397,11 @@
       <c r="C45" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -1153,8 +1411,11 @@
       <c r="C46" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1164,8 +1425,11 @@
       <c r="C47" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1176,7 +1440,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>3</v>
       </c>
@@ -1186,8 +1450,11 @@
       <c r="C49" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -1197,8 +1464,11 @@
       <c r="C50" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1208,8 +1478,11 @@
       <c r="C51" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1219,8 +1492,11 @@
       <c r="C52" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>3</v>
       </c>
@@ -1230,8 +1506,11 @@
       <c r="C53" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1241,8 +1520,11 @@
       <c r="C54" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1252,8 +1534,11 @@
       <c r="C55" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -1264,7 +1549,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>3</v>
       </c>
@@ -1274,8 +1559,11 @@
       <c r="C57" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1285,8 +1573,11 @@
       <c r="C58" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1296,8 +1587,11 @@
       <c r="C59" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1308,7 +1602,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>3</v>
       </c>
@@ -1319,7 +1613,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -1330,7 +1624,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -1341,7 +1635,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>3</v>
       </c>

</xml_diff>